<commit_message>
Add 30 more lines to test data and rerun script
</commit_message>
<xml_diff>
--- a/tests/TestData.xlsx
+++ b/tests/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/jackmyers_microsoft_com/Documents/CELAHACK2023/Teals_Lighthosue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackmyers\repos\FlowiseChatEmbed-main\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="6_{6ED1D574-7E1B-4EE4-83E4-3E012CC26E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A5C2F59-F373-4A1D-8BFB-455A71D976CC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0655974D-FF97-4AAC-B03D-9CB1418BB7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="2964" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="1" xr2:uid="{2ED8FC39-D0CB-4C61-A39F-4C4461D30D05}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{2ED8FC39-D0CB-4C61-A39F-4C4461D30D05}"/>
   </bookViews>
   <sheets>
     <sheet name="DEI Resources" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="249">
   <si>
     <t>DEI Category</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>Question</t>
   </si>
   <si>
     <t>Answer_Location</t>
@@ -517,7 +520,367 @@
     <t>TEALS only works with high schools. We strongly believe computer science is very important for elementary and middle schools, but our program is focused on building teacher capacity at the high-school level, where the curricula require more ramp-up time for the classroom teachers. If your school is interested in starting a middle school program, Microsoft Philanthropies partners with organizations that provide support for elementary and middle schools</t>
   </si>
   <si>
-    <t>Question</t>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>What are microagressions?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - 7 Steps Toward Building an Equitable School Culture _ Edutopia.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Microagressions are “brief, everyday exchanges that send denigrating messages to individuals because of their group membership. The persons making the comments may be otherwise well-intentioned and unaware of the potential impact of their words.</t>
+  </si>
+  <si>
+    <t>Computer code is elegant? How can zeroes and ones be elegant?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Code and Poetry, a Conversation. In which I explore their similarities _ by Angus Croll _ Medium.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Programmers rarely work in zeroes and ones. Their code is written for
+human consumption just as much as for machines. Humans must
+understand code because it’s their job to debug and maintain it—moreover,
+expressive (even beautiful) code is how new idioms proliferate and the
+language evolves._x000D_</t>
+  </si>
+  <si>
+    <t>How can I connect Physical and Virtual Learning Spaces</t>
+  </si>
+  <si>
+    <t>https://microsoft.sharepoint.com/teams/Nonprofit/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=Ehp6Qc&amp;xsdata=MDV8MDF8fDczZDQyY2YxZDhhZDQ5NzBiNTYwMDhkYmYwNWQzMGYyfDk5ZjlmOGU1MmUzNjRiOGU4YmRjZDFiYTUxMTIxYTE3fDB8MHw2MzgzNjgwNTUyNDY4OTQ0MzJ8VW5rbm93bnxWR1ZoYlhOVFpXTjFjbWwwZVZObGNuWnBZMlY4ZXlKV0lqb2lNQzR3TGpBd01EQWlMQ0pRSWpvaVYybHVNeklpTENKQlRpSTZJazkwYUdWeUlpd2lWMVFpT2pFeGZRPT18MXxMMk5vWVhSekx6RTVPalJtTXpFMU1UQTBMVEV6WW1JdE5ETTJNUzFoWmpnM0xUSTBOalZoT1RJME9HWXdOMTlrWkdWaFpHTXpNQzAxTVRZM0xUUTRaVGt0WWpnM05pMDJPVGMxT0dVM04ySTFORFJBZFc1eExtZGliQzV6Y0dGalpYTXZiV1Z6YzJGblpYTXZNVGN3TVRJd09EY3lNekk0TVE9PXw4Y2FmYzQ2ZDI0NWQ0NzgwNTNiMDA4ZGJmMDVkMzBmMHxiNTU1MDFmMDFjY2I0NDVhOGRhZGVmMDUyOGJhMThkMw%3D%3D&amp;sdata=VUdwTFl6ck0ydjlxUXFXdi9DdXlOdXN4R0xkQnR5dll2U25Ma3lybklhZz0%3D&amp;ovuser=72f988bf%2D86f1%2D41af%2D91ab%2D2d7cd011db47%2Cganesh%40microsoft%2Ecom&amp;cid=4e761c4c%2Db45f%2D40bc%2Dbbbd%2Dae16fef9a018&amp;FolderCTID=0x01200072D4916F4267B646BDC73E5CE8487E65&amp;OR=Teams%2DHL&amp;CT=1701378275657&amp;clickparams=eyJBcHBOYW1lIjoiVGVhbXMtRGVza3RvcCIsIkFwcFZlcnNpb24iOiI0OS8yMzExMzAwNDIwMCIsIkhhc0ZlZGVyYXRlZFVzZXIiOmZhbHNlfQ%3D%3D&amp;id=%2Fteams%2FNonprofit%2FShared%20Documents%2FTEALS%2FTEALS%20chatGPT%20Project%2FTEALS%20ChatGPT%20PDFs%2FCollaborative%20Learning%20Spaces%5F%20Classrooms%20That%20Connect%20to%20the%20World%20%5F%20Edutopia%2Epdf&amp;parent=%2Fteams%2FNonprofit%2FShared%20Documents%2FTEALS%2FTEALS%20chatGPT%20Project%2FTEALS%20ChatGPT%20PDFs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The design of a learning space can act as a catalyst to promote collaboration and innovation. Seamless integration
+ of technology into classroom furniture and lessons can empower students to create personalized paths to learning.
+ You can design a collaboration station by moving a flat-edged table to a wall. Chairs surrounding the table will invite
+ student groups to work and collaborate here. An Apple TV added to a mounted flat-screen television lets you mirror
+ devices during project sessions. Physical spaces can then be connected to virtual spaces through creativity and
+ productivity apps. Classrooms can create international learning teams with students of the world, and then use apps-- such as Nearpod
+ (https://www.nearpod.com/)
+ (https://www.google.com/drive/)
+ , and Periscope 
+, Padlet
+ (https://padlet.com/)
+ (https://www.periscope.tv/)
+ , Kahoot!
+ (https://getkahoot.com/)
+ , Google Drive-- in global collaborations and projects.
+ Videoconferencing platforms like Google Hangouts 
+(https://hangouts.google.com/)
+ and Skype in the Classroom allow
+ students to connect to the world through conversations and sharing their stories.</t>
+  </si>
+  <si>
+    <t>What can I do to promote equity and antiracism?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - A Guide to Equity and Antiracism for Educators _ Edutopia.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>You can read or watch to improve your culutral competence and learn about systemic inequities and bias.. You can also take action by creating a personal plan to  support, donate, or volunteer in the way they find most relevant. You also could look within to inventory their feelings to produce change in you over the long-haul.</t>
+  </si>
+  <si>
+    <t>What is the first step for students to become self-aware?</t>
+  </si>
+  <si>
+    <t>How to Get Started Integrating SEL Into Lessons _ Edutopia</t>
+  </si>
+  <si>
+    <t>Naming emotions is a critical first step needed for students to become self-aware and begin to manage their own emotional states effectively—psychologists call this labeling.</t>
+  </si>
+  <si>
+    <t>When dealing with topics involving race where adults don't agree, what should you do?</t>
+  </si>
+  <si>
+    <t>How to Prepare School Staff for Diversity, Equity, and Inclusion Initiatives _ Edutopia</t>
+  </si>
+  <si>
+    <t>When dealing with topics involving race or others where the adults don’t agree (e.g., social justice, emotionally charged current events, systemic racism), it’s critical to establish equity of voice, set ground rules for continued discussions, and define microaggressions in order to develop a school-wide culture of inclusivity that is free from harm for all.</t>
+  </si>
+  <si>
+    <t>What belief does the design of physical spaces communicate?</t>
+  </si>
+  <si>
+    <t>howdoesthephysicalenvironmentaffectwomensentryandpersistenceincomputing</t>
+  </si>
+  <si>
+    <t>The design of physical spaces communicates beliefs about what kinds of people belong in them and what kinds of activities should be done in them (Hattenauer, 1984).</t>
+  </si>
+  <si>
+    <t>What factors suggest TEALS isn't for your school?</t>
+  </si>
+  <si>
+    <t>Is TEALS a good fit for your school</t>
+  </si>
+  <si>
+    <t>1. Your school serves only K-8 students
+2. Your school already has a builtout CS pathway
+3. You want support in a specific CS topic.</t>
+  </si>
+  <si>
+    <t>What is the Learning for Justice project?</t>
+  </si>
+  <si>
+    <t>ISTE _ 10 Resources for Teaching Anti-Racism _ ISTE</t>
+  </si>
+  <si>
+    <t>The Learning for Justice project (formerly Teaching Tolerance) provides a wealth of free resources for K-12 educators to teach tolerance with an emphasis on anti-bias and social justice. It’s Social Justice Standards show how anti-bias education works through the four domains of identity, diversity, justice and action. The project offers lesson plans, teaching strategies and materials including texts, films and posters. It also provides professional development for teachers through workshops, self-guided learning, webinars and podcasts.</t>
+  </si>
+  <si>
+    <t>What are SEL competencies?</t>
+  </si>
+  <si>
+    <t>ISTE _ 3 Ways Teachers Can Integrate SEL Into Learning _ ISTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEL competencies are a guide to show educators how they can help learners understand themselves and others to develop the skills to become better students and people. </t>
+  </si>
+  <si>
+    <t>What are the elements in the Equity and SEL Integration Framework?</t>
+  </si>
+  <si>
+    <t>ISTE _ A New Framework for Activating Equity and SEL in the Classroom</t>
+  </si>
+  <si>
+    <t>1. Understand the CASEL 5.
+2. Assess your own unconscious and implicit biases.
+3. Improve your knowledge of your students.
+4. Help students develop emotional intelligence skills.
+5. Activate SEL in your curriculum</t>
+  </si>
+  <si>
+    <t>What are some frustration-managements strategies?</t>
+  </si>
+  <si>
+    <t>Managing frustration - Supporting Social Participation of All Students</t>
+  </si>
+  <si>
+    <t>- using positive visualization prior to a difficult activity or situation
+- recognizing stress in their bodies and taking time to calm down
+- using self-talk to calm themselves down (e.g., "I am calm" or counting to 10)
+- STAR Strategy (Stop, Take a deep breath And Relax).</t>
+  </si>
+  <si>
+    <t>Is Computer Science for boys?</t>
+  </si>
+  <si>
+    <t>Most Common Myths About Computer Science Debunked</t>
+  </si>
+  <si>
+    <t>This is a common misconception not only in computer science but also in other
+technical fields. Many people believe that computer science is for boys.
+While we can’t deny the fact that computer science is a male-dominated field,
+anyone can get into it and succeed regardless of their gender. There are many
+women who have made incredible inventions in the field of computer science. To
+counter this misconception, there have spirited efforts to encourage more girls to
+enroll in STEM classes.</t>
+  </si>
+  <si>
+    <t>What is wise feedback?</t>
+  </si>
+  <si>
+    <t>NCWIT Tips_ 8 Ways to Give Students More Effective Feedback Using a Growth Mindset _ National Center for Women &amp; Information Technology</t>
+  </si>
+  <si>
+    <t>Students are more likely to make the necessary additional effort if you clearly explain that you are holding them to high standards, that your corrections identify where the students have not yet met those standards, and that your suggestions tell them more about what work at those standards looks like. Finally, and very importantly, clearly express your confidence that the students have the capacity to reach those standards.</t>
+  </si>
+  <si>
+    <t>What's pair programming?</t>
+  </si>
+  <si>
+    <t>Pair Programming_ 10 Cool Tips to Make It Work in Your Classrooms - ETR</t>
+  </si>
+  <si>
+    <t>Pair programming is when two people program on a computer together. Each partner has a different role. One is the “Driver,” controlling the mouse and keyboard. One is the “Navigator,” who helps direct the driver. They complete programming tasks together, rotating roles regularly.</t>
+  </si>
+  <si>
+    <t>What is remote instruction and how does it work?</t>
+  </si>
+  <si>
+    <t>SY22-23-TEALS-School-Growth-Brochure</t>
+  </si>
+  <si>
+    <t>TEALS offers options for remote or inperson volunteer support. Using remote instruction, TEALS volunteers participate using video conferencing software that is chosen by the school. Remote is a great choice for communities with limited local technology professionals</t>
+  </si>
+  <si>
+    <t>What percentae of volunteers said that TEALS was a rewarding experience?</t>
+  </si>
+  <si>
+    <t>TEALS Volunteer information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85% of volunteers said that TEALS was a rewarding experience. </t>
+  </si>
+  <si>
+    <t>What are some tips  that counselor can use to guide students to you CS courses?</t>
+  </si>
+  <si>
+    <t>Top 10 Ways to Engage School Counselors as Allies in the Effort to Increase Student Access to Computer Science Education and Careers _ National Center for Women &amp; Information Technology</t>
+  </si>
+  <si>
+    <t>Tip: Meet with counselors and share an introductory lesson from your curriculum or an “unplugged” activity so they experience computational thinking first hand.
+Tip: The beauty of CS is that it is project-based and results in artifacts of learning that can be shared. Send students to the counseling center to share their projects and excitement about CS.</t>
+  </si>
+  <si>
+    <t>How to optimize individual choie and autonomy?</t>
+  </si>
+  <si>
+    <t>UDL_ Optimize individual choice and autonomy</t>
+  </si>
+  <si>
+    <t>In an instructional setting, it is often inappropriate to provide choice of the learning objective itself, but it is often appropriate to offer choices in how that objective can be reached, in the context for achieving the objective, in the tools or supports available, and so forth. Offering learners choices can develop self-determination, pride in accomplishment, and increase the degree to which they feel connected to their learning. However, it is important to note that individuals differ in how much and what kind of choices they prefer to have. It is therefore not enough to simply provide choice. The right kind of choice and level of independence must be optimized to ensure engagement.</t>
+  </si>
+  <si>
+    <t>How do I set up a circle?</t>
+  </si>
+  <si>
+    <t>Using Circle Practice in the Classroom _ Edutopia</t>
+  </si>
+  <si>
+    <t>Start with the physical space. After years of practice, I have a routine: On my centerpiece—a beautiful round, knitted blanket I received from a colleague—I place a talking piece that acts as a physical signifier indicating whose voice we are listening to at any time. I use a rock, crystal, stuffed animal, or toy. Around the centerpiece are enough chairs for all participants; the chairs must be in close proximity to foster intimacy.
+Next, set up the purpose and expectations. If it’s the first circle with a group, I have an overview printed to use as a guide. I explain the overarching purpose of circle: to form a community with open lines of communication, which is so important to taking intellectual risks.</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>How can you certify a computer professional?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Common Myths _ CityU CS Admission.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>There are various professional certification examinations to certify the professionalism of a computer professional in
+particular skills including software project management, database management and computer security. Although
+someone can become a programmer after self-study on a programming language, formal training of Computer
+Science and related disciplines is highly important for becoming a successful computer professional.</t>
+  </si>
+  <si>
+    <t>Do you need coding experience to study computer science?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Computer Science Recruitment Strategies AP Central _ College Board.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>No, students do not  need any coding experience to begin studying computer science.</t>
+  </si>
+  <si>
+    <t>How can I provide options for recruiting interest?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Copy-of-UDL-and-CS_CT-remix.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Give students choices (choose
+project, software, topic)
+● Allow students to make projects
+relevant to culture and age
+● Minimize possible common “pitfalls”
+for both computing and content
+● Allow for differences in pacing and
+length of work sessions
+● Provide options to increase or
+decrease sensory stimulation (for
+example listening to music with
+headphones or using noise
+cancelling headphones)
+● Allow for differences in pacing and
+length of work sessions</t>
+  </si>
+  <si>
+    <t>What are five things I can do to engage girls in CS?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - CS_Recruitment-Toolkit_Final_update4.23.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can provide role models, generate excitinment, provide hands-on experiences, provide encouragement, and encourage a growth mindset. </t>
+  </si>
+  <si>
+    <t>What is culturally relevant pedagogy?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Culturally relevant pedagogy for computing education - Raspberry Pi Foundation.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Culturally relevant pedagogy is a framework for teaching that emphasises the
+importance of incorporating and valuing all learners’ knowledge, ways of learning,
+and heritage. It promotes the development of learners’ critical consciousness of
+the world and encourages them to ask questions about ethics, power, privilege,
+and social justice. Culturally relevant pedagogy emphasises opportunities to
+address issues that are important to learners and their communities._x000D_</t>
+  </si>
+  <si>
+    <t>Do incidents of hate and bias occur less if adults are present?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Disrupting Your Texts_ Why Simply Including Diverse Voices Is Not Enough.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>A majority of incidents of hate and bias occurred in spaces where adults were present: 32% in classrooms and 37% in shared spaces such as hallways, bathrooms, or other parts of the building.</t>
+  </si>
+  <si>
+    <t>What is DO-IT?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - EA_Computer_Labs.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>DO-IT (Disabilities, Opportunities, 
+Internetworking, and Technology) serves to 
+increase the successful participation of individuals 
+with disabilities in challenging academic 
+programs such as those in science, engineering, 
+mathematics, and technology. Primary funding for 
+the DO-IT program is provided by the National 
+Science Foundation, the State of Washington, and 
+the U.S. Department of Education.</t>
+  </si>
+  <si>
+    <t>What are tips for promoting equity in the classroom?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - EquityStrategies.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Some tips are to decorate with purpose, make eye contact, call on everyone, take your time, cut back on homework, show instead of just telling, provided access to all students, providing a coment box, and being available to your students.</t>
+  </si>
+  <si>
+    <t>What is a growth mindset?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Girls_In_STEM Whitepaper.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>A“growth mindset,” is defined by Stanford professor Carol 
+Dweck as one that is focused on continual 
+learning and improvement, through a willingness 
+to try, fail and inquire</t>
+  </si>
+  <si>
+    <t>How is identity helpful for students transitioning into a new culture?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - Harnessing the Power of Storytelling to Support Migrant and Immigrant Students in Middle and High School _ Edutopia.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Identifying different layers of identity, like individual characteristics, Microsystem, Exosystem, and Macrosystem,  is particularly helpful for newcomers looking to develop their identities. Helping these students isolate the changes in the relationship between their identities and their environment can help them navigate the challenges of living in a new land.</t>
+  </si>
+  <si>
+    <t>How can I begin with empathy mapping?</t>
+  </si>
+  <si>
+    <t>Philanthropies Engineering &amp; Ops Collab - How Empathy Maps Can Help Teachers Connect With Middle and High School Students _ Edutopia.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Creating empathy maps is relatively simple once you gather pertinent information about your students. This may
+include their goals, hobbies, interests, and areas of academic, career, and social needs, as well as data from
+assessments. Traditional ways of collecting this information about students can be through polls, surveys, and
+looking at student work (e.g., reflection journals, essays, digital portfolios, and passion-project-based learning
+projects). Knowledge about students can also be gleaned in classroom discussions aimed at checking in and
+building rapport, paying attention to what they care about (e.g., social issues), recognizing their gifts and abilities in
+how they transfer learning and in things they voluntarily talk about. You should  update this data throughout the school year to keep up as kids change.</t>
   </si>
 </sst>
 </file>
@@ -545,7 +908,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,10 +921,45 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -572,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -584,6 +982,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -665,8 +1076,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BFA754B-7F8F-4BDE-B231-AFBA88F33482}" name="Table2" displayName="Table2" ref="A1:D23" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D23" xr:uid="{3BFA754B-7F8F-4BDE-B231-AFBA88F33482}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BFA754B-7F8F-4BDE-B231-AFBA88F33482}" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D25" xr:uid="{3BFA754B-7F8F-4BDE-B231-AFBA88F33482}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C0874798-B028-4B7E-8A27-262EFD75D0B0}" name="User" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{710FBF78-80FF-484B-BC58-C6A5802025DE}" name="Question" dataDxfId="2"/>
@@ -1707,17 +2118,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EACD4E-6A4B-447C-B57B-1BDB449FFCE0}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="107.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1727,331 +2138,787 @@
         <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C22" r:id="rId1" xr:uid="{88FA9579-A0FF-4D7C-9076-1B30E9A04514}"/>
     <hyperlink ref="C7" r:id="rId2" xr:uid="{BB6E1B43-DEC5-4119-879B-91595D2E22D7}"/>
+    <hyperlink ref="C23" r:id="rId3" xr:uid="{2817A61F-6953-4268-9F88-D9B488BC9908}"/>
+    <hyperlink ref="C26" r:id="rId4" xr:uid="{04B8F5D0-3437-4C31-9D6C-C169CA0EF482}"/>
+    <hyperlink ref="C27" r:id="rId5" xr:uid="{3386A1C1-458E-4976-9486-38C6AFC7FFEC}"/>
+    <hyperlink ref="C28" r:id="rId6" xr:uid="{49403410-09C4-4ACC-91A5-7B649144EC16}"/>
+    <hyperlink ref="C29" r:id="rId7" xr:uid="{515B1224-C51E-44B0-B5B9-40EDB3EA5AA5}"/>
+    <hyperlink ref="C30" r:id="rId8" xr:uid="{FDCBB567-6ABF-4C14-B78E-E2E8A2D0DC82}"/>
+    <hyperlink ref="C31" r:id="rId9" xr:uid="{D1D2BAB4-3E3A-41B1-A560-278B8C86E2D2}"/>
+    <hyperlink ref="C32" r:id="rId10" xr:uid="{C32FE84E-6F27-4DEF-9B2B-0AC30F341881}"/>
+    <hyperlink ref="C33" r:id="rId11" xr:uid="{9DECBD1E-CDC1-4E2F-9913-E2AEB8296740}"/>
+    <hyperlink ref="C34" r:id="rId12" xr:uid="{7A5C0BA3-AB6D-4ABE-BAC4-D9FBF13BF0A6}"/>
+    <hyperlink ref="C35" r:id="rId13" xr:uid="{5CBCA215-6558-4E61-A042-EEBCEE4DA20A}"/>
+    <hyperlink ref="C36" r:id="rId14" xr:uid="{4BE9ED08-4653-443C-B5E0-F3E8682D7083}"/>
+    <hyperlink ref="C37" r:id="rId15" xr:uid="{30D34B27-DA30-4260-A410-CAC5A7A45D19}"/>
+    <hyperlink ref="C38" r:id="rId16" xr:uid="{9D4846C8-9F8C-47AE-9E68-F4FC735E1159}"/>
+    <hyperlink ref="C39" r:id="rId17" xr:uid="{05EDA1BA-62BF-43F0-A5AA-58A2CE4253F9}"/>
+    <hyperlink ref="C40" r:id="rId18" xr:uid="{DCC021C5-03F4-4F22-9049-270A4B6C96BF}"/>
+    <hyperlink ref="C41" r:id="rId19" xr:uid="{59452DCB-CC4A-4F9B-8AD1-331A10D92650}"/>
+    <hyperlink ref="C42" r:id="rId20" xr:uid="{76B16240-1FCA-427A-9F52-E0F3786C086E}"/>
+    <hyperlink ref="C24" r:id="rId21" xr:uid="{87339512-AF02-4159-942D-ECDFCEB2D798}"/>
+    <hyperlink ref="C25" r:id="rId22" display="https://microsoft.sharepoint.com/teams/Nonprofit/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=Ehp6Qc&amp;xsdata=MDV8MDF8fDczZDQyY2YxZDhhZDQ5NzBiNTYwMDhkYmYwNWQzMGYyfDk5ZjlmOGU1MmUzNjRiOGU4YmRjZDFiYTUxMTIxYTE3fDB8MHw2MzgzNjgwNTUyNDY4OTQ0MzJ8VW5rbm93bnxWR1ZoYlhOVFpXTjFjbWwwZVZObGNuWnBZMlY4ZXlKV0lqb2lNQzR3TGpBd01EQWlMQ0pRSWpvaVYybHVNeklpTENKQlRpSTZJazkwYUdWeUlpd2lWMVFpT2pFeGZRPT18MXxMMk5vWVhSekx6RTVPalJtTXpFMU1UQTBMVEV6WW1JdE5ETTJNUzFoWmpnM0xUSTBOalZoT1RJME9HWXdOMTlrWkdWaFpHTXpNQzAxTVRZM0xUUTRaVGt0WWpnM05pMDJPVGMxT0dVM04ySTFORFJBZFc1eExtZGliQzV6Y0dGalpYTXZiV1Z6YzJGblpYTXZNVGN3TVRJd09EY3lNekk0TVE9PXw4Y2FmYzQ2ZDI0NWQ0NzgwNTNiMDA4ZGJmMDVkMzBmMHxiNTU1MDFmMDFjY2I0NDVhOGRhZGVmMDUyOGJhMThkMw%3D%3D&amp;sdata=VUdwTFl6ck0ydjlxUXFXdi9DdXlOdXN4R0xkQnR5dll2U25Ma3lybklhZz0%3D&amp;ovuser=72f988bf%2D86f1%2D41af%2D91ab%2D2d7cd011db47%2Cganesh%40microsoft%2Ecom&amp;cid=4e761c4c%2Db45f%2D40bc%2Dbbbd%2Dae16fef9a018&amp;FolderCTID=0x01200072D4916F4267B646BDC73E5CE8487E65&amp;OR=Teams%2DHL&amp;CT=1701378275657&amp;clickparams=eyJBcHBOYW1lIjoiVGVhbXMtRGVza3RvcCIsIkFwcFZlcnNpb24iOiI0OS8yMzExMzAwNDIwMCIsIkhhc0ZlZGVyYXRlZFVzZXIiOmZhbHNlfQ%3D%3D&amp;id=%2Fteams%2FNonprofit%2FShared%20Documents%2FTEALS%2FTEALS%20chatGPT%20Project%2FTEALS%20ChatGPT%20PDFs%2FCollaborative%20Learning%20Spaces%5F%20Classrooms%20That%20Connect%20to%20the%20World%20%5F%20Edutopia%2Epdf&amp;parent=%2Fteams%2FNonprofit%2FShared%20Documents%2FTEALS%2FTEALS%20chatGPT%20Project%2FTEALS%20ChatGPT%20PDFs" xr:uid="{88F7B8DB-6E6E-4A11-A63C-F4642BC42506}"/>
+    <hyperlink ref="C43" r:id="rId23" xr:uid="{90149A6A-2073-49C0-AF83-6400C8B1ABE2}"/>
+    <hyperlink ref="C44" r:id="rId24" xr:uid="{5ABC8038-61D8-45AD-87ED-D7B9C778E9FF}"/>
+    <hyperlink ref="C45" r:id="rId25" xr:uid="{0A38EFF8-CD12-4C22-81D5-1ECBD0A1C606}"/>
+    <hyperlink ref="C46" r:id="rId26" xr:uid="{5CB1FA3A-E4EE-44DE-864E-F28DAE1E9D2B}"/>
+    <hyperlink ref="C47" r:id="rId27" xr:uid="{6009ED97-56BE-4526-856F-B347BD369038}"/>
+    <hyperlink ref="C48" r:id="rId28" xr:uid="{AB40E6D4-CB25-4507-AC7D-B4A7C564317C}"/>
+    <hyperlink ref="C49" r:id="rId29" xr:uid="{A402A38E-A4CC-4251-9920-2339BBF9C956}"/>
+    <hyperlink ref="C50" r:id="rId30" xr:uid="{6D381B29-33A9-45A0-A3D5-13BEECD52DA6}"/>
+    <hyperlink ref="C51" r:id="rId31" xr:uid="{7BC3DECA-E3EF-47CA-8E23-D07560D9C931}"/>
+    <hyperlink ref="C52" r:id="rId32" xr:uid="{EBBC3F4B-90A0-44CD-BB0C-31830EFB5214}"/>
+    <hyperlink ref="C53" r:id="rId33" xr:uid="{096D164F-08BD-4654-AE6C-D3C1C1069BC6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003E6277BB0039B747B9A05DD8F711D89B" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c71c00e7c3ae997f5b04a0adc9923301">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7e9b50db-29be-493e-9f23-16304e4e8518" xmlns:ns3="aca2a79c-eca5-45ac-ae12-75019d339679" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c619e1f77f59e46e0974bd914b9ccb45" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2348,6 +3215,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2366,14 +3242,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFFE82EC-1CB9-49FD-86BC-486220DC51CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C700C6-9B6C-4FA6-B07B-BCAED10B26B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2390,6 +3258,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFFE82EC-1CB9-49FD-86BC-486220DC51CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>